<commit_message>
added new X0 value and heat ploting code
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaktimukker/Documents/MyProjects/projects/bacterial-growth-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F855BBA-477C-634C-AD71-A866DE3461F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86246F7A-C097-F943-B56E-320E47FBE0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="train" sheetId="5" r:id="rId1"/>
@@ -1765,10 +1765,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC4FC5FB-8DD8-CC48-9415-894A26C06305}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1786,7 +1786,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>9.9999999999999982</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1794,7 +1794,7 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>12.321428571428571</v>
+        <v>12.32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1802,7 +1802,7 @@
         <v>24</v>
       </c>
       <c r="B4">
-        <v>17.142857142857139</v>
+        <v>17.14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1810,7 +1810,7 @@
         <v>32</v>
       </c>
       <c r="B5">
-        <v>21.071428571428569</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1818,7 +1818,7 @@
         <v>40</v>
       </c>
       <c r="B6">
-        <v>12.5</v>
+        <v>21.87</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1826,7 +1826,7 @@
         <v>48</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>22.67</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1834,7 +1834,7 @@
         <v>56</v>
       </c>
       <c r="B8">
-        <v>23.928571428571427</v>
+        <v>23.92</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1842,7 +1842,7 @@
         <v>64</v>
       </c>
       <c r="B9">
-        <v>20.714285714285712</v>
+        <v>22.71</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1850,7 +1850,7 @@
         <v>72</v>
       </c>
       <c r="B10">
-        <v>21.249999999999996</v>
+        <v>22.25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1858,7 +1858,7 @@
         <v>80</v>
       </c>
       <c r="B11">
-        <v>16.071428571428569</v>
+        <v>22.32</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1866,7 +1866,7 @@
         <v>88</v>
       </c>
       <c r="B12">
-        <v>18.928571428571423</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1874,7 +1874,7 @@
         <v>96</v>
       </c>
       <c r="B13">
-        <v>23.035714285714285</v>
+        <v>20.03</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1882,7 +1882,7 @@
         <v>104</v>
       </c>
       <c r="B14">
-        <v>15.535714285714283</v>
+        <v>20.350000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1890,7 +1890,7 @@
         <v>112</v>
       </c>
       <c r="B15">
-        <v>18.749999999999996</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1898,7 +1898,7 @@
         <v>120</v>
       </c>
       <c r="B16">
-        <v>20.357142857142858</v>
+        <v>16.07</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1906,47 +1906,7 @@
         <v>128</v>
       </c>
       <c r="B17">
-        <v>18.571428571428569</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>136</v>
-      </c>
-      <c r="B18">
-        <v>16.071428571428569</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>144</v>
-      </c>
-      <c r="B19">
-        <v>17.857142857142858</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>152</v>
-      </c>
-      <c r="B20">
-        <v>22.678571428571423</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>160</v>
-      </c>
-      <c r="B21">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>168</v>
-      </c>
-      <c r="B22">
-        <v>22.499999999999996</v>
+        <v>15.53</v>
       </c>
     </row>
   </sheetData>
@@ -1958,7 +1918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6277E3-AFF1-FA45-9062-E213A9069154}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>